<commit_message>
Updated the Course List
</commit_message>
<xml_diff>
--- a/util/report_chennai.xlsx
+++ b/util/report_chennai.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harik\OneDrive\Pictures\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E96936D-17FA-4089-AFD6-6C7E11DD674A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45990030-06C2-43C3-9FB8-D58D936C5F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2641" uniqueCount="527">
   <si>
     <t>VENUE</t>
   </si>
@@ -1461,13 +1461,157 @@
   </si>
   <si>
     <t>L1+L2+L9+L10+L21+L22</t>
+  </si>
+  <si>
+    <t>BINU BEN JOSE D R</t>
+  </si>
+  <si>
+    <t>G1 + TG1</t>
+  </si>
+  <si>
+    <t>MEERA P S</t>
+  </si>
+  <si>
+    <t>G2 + TG2</t>
+  </si>
+  <si>
+    <t>KANIMOZHI G</t>
+  </si>
+  <si>
+    <t>HEMAMALINI</t>
+  </si>
+  <si>
+    <t>LAVANYA V</t>
+  </si>
+  <si>
+    <t>JAMUNA K</t>
+  </si>
+  <si>
+    <t>MOHAMED IMRAN A</t>
+  </si>
+  <si>
+    <t>PREMALATHA L</t>
+  </si>
+  <si>
+    <t>DEEPA T</t>
+  </si>
+  <si>
+    <t>C1 + TC1</t>
+  </si>
+  <si>
+    <t>NITHYA VENKATESAN</t>
+  </si>
+  <si>
+    <t>SENTHIL KUMAR N</t>
+  </si>
+  <si>
+    <t>FEBIN DAYA J L</t>
+  </si>
+  <si>
+    <t>ANGELINE EZHILARASI</t>
+  </si>
+  <si>
+    <t>CHENDHUR KUMARAN R</t>
+  </si>
+  <si>
+    <t>SUBBULEKSHMI D</t>
+  </si>
+  <si>
+    <t>SRIMATHI R</t>
+  </si>
+  <si>
+    <t>C2 + TC2</t>
+  </si>
+  <si>
+    <t>SASIPRIYA P</t>
+  </si>
+  <si>
+    <t>HEMALINI</t>
+  </si>
+  <si>
+    <t>L43 + L44</t>
+  </si>
+  <si>
+    <t>L11 + L12</t>
+  </si>
+  <si>
+    <t>L55 + L56</t>
+  </si>
+  <si>
+    <t>L:15 + L16</t>
+  </si>
+  <si>
+    <t>L37 + L38</t>
+  </si>
+  <si>
+    <t>L13 + L14</t>
+  </si>
+  <si>
+    <t>L49 + L50</t>
+  </si>
+  <si>
+    <t>L7 + L8</t>
+  </si>
+  <si>
+    <t>L25 + L26</t>
+  </si>
+  <si>
+    <t>L9 + L10</t>
+  </si>
+  <si>
+    <t>L31 + L32</t>
+  </si>
+  <si>
+    <t>KURUSEELAN S</t>
+  </si>
+  <si>
+    <t>L19 + L20</t>
+  </si>
+  <si>
+    <t>L33 + L34</t>
+  </si>
+  <si>
+    <t>L27 + L28</t>
+  </si>
+  <si>
+    <t>L51 + L52</t>
+  </si>
+  <si>
+    <t>L23 + L24</t>
+  </si>
+  <si>
+    <t>L57 + L58</t>
+  </si>
+  <si>
+    <t>L1 + L2</t>
+  </si>
+  <si>
+    <t>L45 + L46</t>
+  </si>
+  <si>
+    <t>L21 + L22</t>
+  </si>
+  <si>
+    <t>SRI REVATHI B</t>
+  </si>
+  <si>
+    <t>:L3 + L4</t>
+  </si>
+  <si>
+    <t>M. PRABHAKAR</t>
+  </si>
+  <si>
+    <t>ISWARYA ANNAPOORANI</t>
+  </si>
+  <si>
+    <t>L39 + L40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1517,6 +1661,12 @@
     <font>
       <sz val="14"/>
       <color rgb="FF212529"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF343A40"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1642,9 +1792,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1652,6 +1799,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1994,10 +2144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G929"/>
+  <dimension ref="A1:G931"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A447" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="G426" sqref="G426"/>
+    <sheetView tabSelected="1" topLeftCell="A480" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A494" sqref="A494"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.296875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -10026,7 +10176,7 @@
       </c>
     </row>
     <row r="422" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A422" s="15" t="s">
+      <c r="A422" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B422" s="7" t="s">
@@ -10037,7 +10187,7 @@
       </c>
       <c r="D422" s="7"/>
       <c r="E422" s="7"/>
-      <c r="F422" s="17" t="s">
+      <c r="F422" s="16" t="s">
         <v>445</v>
       </c>
       <c r="G422" s="7" t="s">
@@ -10045,7 +10195,7 @@
       </c>
     </row>
     <row r="423" spans="1:7" ht="44.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A423" s="15" t="s">
+      <c r="A423" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B423" s="7" t="s">
@@ -10064,7 +10214,7 @@
       </c>
     </row>
     <row r="424" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A424" s="15" t="s">
+      <c r="A424" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B424" s="7" t="s">
@@ -10073,7 +10223,7 @@
       <c r="C424" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D424" s="16"/>
+      <c r="D424" s="15"/>
       <c r="E424" s="7"/>
       <c r="F424" s="7" t="s">
         <v>448</v>
@@ -10083,7 +10233,7 @@
       </c>
     </row>
     <row r="425" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A425" s="15" t="s">
+      <c r="A425" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B425" s="7" t="s">
@@ -10092,7 +10242,7 @@
       <c r="C425" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D425" s="16"/>
+      <c r="D425" s="15"/>
       <c r="E425" s="7"/>
       <c r="F425" s="7" t="s">
         <v>449</v>
@@ -10102,7 +10252,7 @@
       </c>
     </row>
     <row r="426" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A426" s="15" t="s">
+      <c r="A426" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B426" s="7" t="s">
@@ -10111,7 +10261,7 @@
       <c r="C426" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D426" s="16"/>
+      <c r="D426" s="15"/>
       <c r="E426" s="7"/>
       <c r="F426" s="7" t="s">
         <v>447</v>
@@ -10121,7 +10271,7 @@
       </c>
     </row>
     <row r="427" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A427" s="15" t="s">
+      <c r="A427" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B427" s="7" t="s">
@@ -10130,7 +10280,7 @@
       <c r="C427" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D427" s="16"/>
+      <c r="D427" s="15"/>
       <c r="E427" s="7"/>
       <c r="F427" s="7" t="s">
         <v>453</v>
@@ -10140,7 +10290,7 @@
       </c>
     </row>
     <row r="428" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A428" s="15" t="s">
+      <c r="A428" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B428" s="7" t="s">
@@ -10149,7 +10299,7 @@
       <c r="C428" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D428" s="16"/>
+      <c r="D428" s="15"/>
       <c r="E428" s="7"/>
       <c r="F428" s="7" t="s">
         <v>454</v>
@@ -10159,7 +10309,7 @@
       </c>
     </row>
     <row r="429" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A429" s="15" t="s">
+      <c r="A429" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B429" s="7" t="s">
@@ -10168,7 +10318,7 @@
       <c r="C429" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D429" s="16"/>
+      <c r="D429" s="15"/>
       <c r="E429" s="7"/>
       <c r="F429" s="7" t="s">
         <v>460</v>
@@ -10178,7 +10328,7 @@
       </c>
     </row>
     <row r="430" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A430" s="15" t="s">
+      <c r="A430" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B430" s="7" t="s">
@@ -10187,7 +10337,7 @@
       <c r="C430" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D430" s="16"/>
+      <c r="D430" s="15"/>
       <c r="E430" s="7"/>
       <c r="F430" s="7" t="s">
         <v>454</v>
@@ -10197,7 +10347,7 @@
       </c>
     </row>
     <row r="431" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A431" s="15" t="s">
+      <c r="A431" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B431" s="7" t="s">
@@ -10206,7 +10356,7 @@
       <c r="C431" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D431" s="16"/>
+      <c r="D431" s="15"/>
       <c r="E431" s="7"/>
       <c r="F431" s="7" t="s">
         <v>456</v>
@@ -10216,7 +10366,7 @@
       </c>
     </row>
     <row r="432" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A432" s="15" t="s">
+      <c r="A432" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B432" s="7" t="s">
@@ -10225,7 +10375,7 @@
       <c r="C432" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D432" s="16"/>
+      <c r="D432" s="15"/>
       <c r="E432" s="7"/>
       <c r="F432" s="7" t="s">
         <v>462</v>
@@ -10235,7 +10385,7 @@
       </c>
     </row>
     <row r="433" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A433" s="15" t="s">
+      <c r="A433" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B433" s="7" t="s">
@@ -10244,7 +10394,7 @@
       <c r="C433" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D433" s="16"/>
+      <c r="D433" s="15"/>
       <c r="E433" s="7"/>
       <c r="F433" s="7" t="s">
         <v>448</v>
@@ -10254,7 +10404,7 @@
       </c>
     </row>
     <row r="434" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A434" s="15" t="s">
+      <c r="A434" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B434" s="7" t="s">
@@ -10263,7 +10413,7 @@
       <c r="C434" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D434" s="16"/>
+      <c r="D434" s="15"/>
       <c r="E434" s="7"/>
       <c r="F434" s="7" t="s">
         <v>449</v>
@@ -10273,7 +10423,7 @@
       </c>
     </row>
     <row r="435" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A435" s="15" t="s">
+      <c r="A435" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B435" s="7" t="s">
@@ -10282,7 +10432,7 @@
       <c r="C435" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D435" s="16"/>
+      <c r="D435" s="15"/>
       <c r="E435" s="7"/>
       <c r="F435" s="7" t="s">
         <v>466</v>
@@ -10292,7 +10442,7 @@
       </c>
     </row>
     <row r="436" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A436" s="15" t="s">
+      <c r="A436" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B436" s="7" t="s">
@@ -10301,7 +10451,7 @@
       <c r="C436" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D436" s="16"/>
+      <c r="D436" s="15"/>
       <c r="E436" s="7"/>
       <c r="F436" s="7" t="s">
         <v>465</v>
@@ -10311,7 +10461,7 @@
       </c>
     </row>
     <row r="437" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A437" s="15" t="s">
+      <c r="A437" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B437" s="7" t="s">
@@ -10320,7 +10470,7 @@
       <c r="C437" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D437" s="16"/>
+      <c r="D437" s="15"/>
       <c r="E437" s="7"/>
       <c r="F437" s="7" t="s">
         <v>466</v>
@@ -10330,7 +10480,7 @@
       </c>
     </row>
     <row r="438" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A438" s="15" t="s">
+      <c r="A438" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B438" s="7" t="s">
@@ -10339,7 +10489,7 @@
       <c r="C438" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D438" s="16"/>
+      <c r="D438" s="15"/>
       <c r="E438" s="7"/>
       <c r="F438" s="7" t="s">
         <v>460</v>
@@ -10349,7 +10499,7 @@
       </c>
     </row>
     <row r="439" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A439" s="15" t="s">
+      <c r="A439" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B439" s="7" t="s">
@@ -10358,7 +10508,7 @@
       <c r="C439" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D439" s="16"/>
+      <c r="D439" s="15"/>
       <c r="E439" s="7"/>
       <c r="F439" s="7" t="s">
         <v>456</v>
@@ -10368,7 +10518,7 @@
       </c>
     </row>
     <row r="440" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A440" s="15" t="s">
+      <c r="A440" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B440" s="7" t="s">
@@ -10377,7 +10527,7 @@
       <c r="C440" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D440" s="16"/>
+      <c r="D440" s="15"/>
       <c r="E440" s="7"/>
       <c r="F440" s="7" t="s">
         <v>454</v>
@@ -10387,7 +10537,7 @@
       </c>
     </row>
     <row r="441" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A441" s="15" t="s">
+      <c r="A441" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B441" s="7" t="s">
@@ -10396,7 +10546,7 @@
       <c r="C441" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D441" s="16"/>
+      <c r="D441" s="15"/>
       <c r="E441" s="7"/>
       <c r="F441" s="7" t="s">
         <v>462</v>
@@ -10406,7 +10556,7 @@
       </c>
     </row>
     <row r="442" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A442" s="15" t="s">
+      <c r="A442" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B442" s="7" t="s">
@@ -10415,7 +10565,7 @@
       <c r="C442" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D442" s="16"/>
+      <c r="D442" s="15"/>
       <c r="E442" s="7"/>
       <c r="F442" s="7" t="s">
         <v>448</v>
@@ -10425,7 +10575,7 @@
       </c>
     </row>
     <row r="443" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A443" s="15" t="s">
+      <c r="A443" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B443" s="7" t="s">
@@ -10434,7 +10584,7 @@
       <c r="C443" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D443" s="16"/>
+      <c r="D443" s="15"/>
       <c r="E443" s="7"/>
       <c r="F443" s="7" t="s">
         <v>460</v>
@@ -10444,7 +10594,7 @@
       </c>
     </row>
     <row r="444" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A444" s="15" t="s">
+      <c r="A444" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B444" s="7" t="s">
@@ -10453,7 +10603,7 @@
       <c r="C444" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D444" s="16"/>
+      <c r="D444" s="15"/>
       <c r="E444" s="7"/>
       <c r="F444" s="7" t="s">
         <v>466</v>
@@ -10463,7 +10613,7 @@
       </c>
     </row>
     <row r="445" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A445" s="15" t="s">
+      <c r="A445" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B445" s="7" t="s">
@@ -10472,7 +10622,7 @@
       <c r="C445" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D445" s="16"/>
+      <c r="D445" s="15"/>
       <c r="E445" s="7"/>
       <c r="F445" s="7" t="s">
         <v>447</v>
@@ -10482,7 +10632,7 @@
       </c>
     </row>
     <row r="446" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A446" s="15" t="s">
+      <c r="A446" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B446" s="7" t="s">
@@ -10491,7 +10641,7 @@
       <c r="C446" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D446" s="16"/>
+      <c r="D446" s="15"/>
       <c r="E446" s="7"/>
       <c r="F446" s="7" t="s">
         <v>462</v>
@@ -10501,7 +10651,7 @@
       </c>
     </row>
     <row r="447" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A447" s="15" t="s">
+      <c r="A447" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B447" s="7" t="s">
@@ -10510,7 +10660,7 @@
       <c r="C447" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D447" s="16"/>
+      <c r="D447" s="15"/>
       <c r="E447" s="7"/>
       <c r="F447" s="7" t="s">
         <v>453</v>
@@ -10520,7 +10670,7 @@
       </c>
     </row>
     <row r="448" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A448" s="15" t="s">
+      <c r="A448" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B448" s="7" t="s">
@@ -10529,7 +10679,7 @@
       <c r="C448" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D448" s="16"/>
+      <c r="D448" s="15"/>
       <c r="E448" s="7"/>
       <c r="F448" s="7" t="s">
         <v>453</v>
@@ -10539,7 +10689,7 @@
       </c>
     </row>
     <row r="449" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A449" s="15" t="s">
+      <c r="A449" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B449" s="7" t="s">
@@ -10548,7 +10698,7 @@
       <c r="C449" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D449" s="16"/>
+      <c r="D449" s="15"/>
       <c r="E449" s="7"/>
       <c r="F449" s="7" t="s">
         <v>466</v>
@@ -10558,7 +10708,7 @@
       </c>
     </row>
     <row r="450" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A450" s="15" t="s">
+      <c r="A450" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B450" s="7" t="s">
@@ -10567,7 +10717,7 @@
       <c r="C450" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D450" s="16"/>
+      <c r="D450" s="15"/>
       <c r="E450" s="7"/>
       <c r="F450" s="7" t="s">
         <v>449</v>
@@ -10577,7 +10727,7 @@
       </c>
     </row>
     <row r="451" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A451" s="15" t="s">
+      <c r="A451" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B451" s="7" t="s">
@@ -10586,7 +10736,7 @@
       <c r="C451" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D451" s="16"/>
+      <c r="D451" s="15"/>
       <c r="E451" s="7"/>
       <c r="F451" s="7" t="s">
         <v>478</v>
@@ -10596,402 +10746,822 @@
       </c>
     </row>
     <row r="452" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A452" s="7"/>
-      <c r="B452" s="7"/>
-      <c r="C452" s="14"/>
-      <c r="D452" s="16"/>
+      <c r="A452" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B452" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C452" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D452" s="15"/>
       <c r="E452" s="7"/>
-      <c r="F452" s="7"/>
-      <c r="G452" s="7"/>
+      <c r="F452" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G452" s="17" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="453" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A453" s="7"/>
-      <c r="B453" s="7"/>
-      <c r="C453" s="7"/>
+      <c r="A453" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B453" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C453" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D453" s="7"/>
       <c r="E453" s="7"/>
-      <c r="F453" s="7"/>
-      <c r="G453" s="7"/>
+      <c r="F453" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="G453" s="7" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="454" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A454" s="7"/>
-      <c r="B454" s="7"/>
-      <c r="C454" s="7"/>
+      <c r="A454" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B454" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C454" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D454" s="7"/>
       <c r="E454" s="7"/>
-      <c r="F454" s="7"/>
-      <c r="G454" s="7"/>
-    </row>
-    <row r="455" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A455" s="7"/>
-      <c r="B455" s="7"/>
-      <c r="C455" s="7"/>
+      <c r="F454" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G454" s="17" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="455" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A455" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B455" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C455" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D455" s="7"/>
       <c r="E455" s="7"/>
-      <c r="F455" s="7"/>
-      <c r="G455" s="7"/>
+      <c r="F455" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G455" s="7" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="456" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A456" s="7"/>
-      <c r="B456" s="7"/>
-      <c r="C456" s="7"/>
+      <c r="A456" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B456" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C456" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D456" s="7"/>
       <c r="E456" s="7"/>
-      <c r="F456" s="7"/>
-      <c r="G456" s="7"/>
+      <c r="F456" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="G456" s="7" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="457" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A457" s="7"/>
-      <c r="B457" s="7"/>
-      <c r="C457" s="7"/>
+      <c r="A457" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B457" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C457" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D457" s="7"/>
       <c r="E457" s="7"/>
-      <c r="F457" s="7"/>
-      <c r="G457" s="7"/>
+      <c r="F457" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G457" s="7" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="458" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A458" s="7"/>
-      <c r="B458" s="7"/>
-      <c r="C458" s="7"/>
+      <c r="A458" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B458" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C458" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D458" s="7"/>
       <c r="E458" s="7"/>
-      <c r="F458" s="7"/>
-      <c r="G458" s="7"/>
+      <c r="F458" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="G458" s="7" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="459" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A459" s="7"/>
-      <c r="B459" s="7"/>
-      <c r="C459" s="7"/>
+      <c r="A459" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B459" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C459" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D459" s="7"/>
       <c r="E459" s="7"/>
-      <c r="F459" s="7"/>
-      <c r="G459" s="7"/>
+      <c r="F459" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="G459" s="7" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="460" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A460" s="7"/>
-      <c r="B460" s="7"/>
-      <c r="C460" s="7"/>
+      <c r="A460" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B460" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C460" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D460" s="7"/>
       <c r="E460" s="7"/>
-      <c r="F460" s="7"/>
-      <c r="G460" s="7"/>
+      <c r="F460" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="G460" s="7" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="461" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A461" s="7"/>
-      <c r="B461" s="7"/>
-      <c r="C461" s="7"/>
+      <c r="A461" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B461" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C461" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D461" s="7"/>
       <c r="E461" s="7"/>
-      <c r="F461" s="7"/>
-      <c r="G461" s="7"/>
+      <c r="F461" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="G461" s="7" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="462" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A462" s="7"/>
-      <c r="B462" s="7"/>
-      <c r="C462" s="7"/>
+      <c r="A462" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B462" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C462" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D462" s="7"/>
       <c r="E462" s="7"/>
-      <c r="F462" s="7"/>
-      <c r="G462" s="7"/>
+      <c r="F462" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G462" s="7" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="463" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A463" s="7"/>
-      <c r="B463" s="7"/>
-      <c r="C463" s="7"/>
+      <c r="A463" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B463" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C463" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D463" s="7"/>
       <c r="E463" s="7"/>
-      <c r="F463" s="7"/>
-      <c r="G463" s="7"/>
+      <c r="F463" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="G463" s="7" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="464" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A464" s="7"/>
-      <c r="B464" s="7"/>
-      <c r="C464" s="7"/>
+      <c r="A464" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B464" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C464" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D464" s="7"/>
       <c r="E464" s="7"/>
-      <c r="F464" s="7"/>
-      <c r="G464" s="7"/>
+      <c r="F464" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G464" s="7" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="465" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A465" s="7"/>
-      <c r="B465" s="7"/>
-      <c r="C465" s="7"/>
+      <c r="A465" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B465" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C465" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D465" s="7"/>
       <c r="E465" s="7"/>
-      <c r="F465" s="7"/>
-      <c r="G465" s="7"/>
+      <c r="F465" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G465" s="7" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="466" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A466" s="7"/>
-      <c r="B466" s="7"/>
-      <c r="C466" s="7"/>
+      <c r="A466" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B466" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C466" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D466" s="7"/>
       <c r="E466" s="7"/>
-      <c r="F466" s="7"/>
-      <c r="G466" s="7"/>
+      <c r="F466" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G466" s="7" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="467" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A467" s="7"/>
-      <c r="B467" s="7"/>
-      <c r="C467" s="7"/>
+      <c r="A467" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B467" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C467" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D467" s="7"/>
       <c r="E467" s="7"/>
-      <c r="F467" s="7"/>
-      <c r="G467" s="7"/>
+      <c r="F467" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G467" s="7" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="468" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A468" s="7"/>
-      <c r="B468" s="7"/>
-      <c r="C468" s="7"/>
+      <c r="A468" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B468" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C468" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D468" s="7"/>
       <c r="E468" s="7"/>
-      <c r="F468" s="7"/>
-      <c r="G468" s="7"/>
-    </row>
-    <row r="469" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A469" s="7"/>
-      <c r="B469" s="7"/>
-      <c r="C469" s="7"/>
+      <c r="F468" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="G468" s="7" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="469" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A469" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B469" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C469" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D469" s="7"/>
       <c r="E469" s="7"/>
-      <c r="F469" s="7"/>
-      <c r="G469" s="7"/>
-    </row>
-    <row r="470" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A470" s="7"/>
-      <c r="B470" s="7"/>
-      <c r="C470" s="7"/>
+      <c r="F469" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="G469" s="7" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="470" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A470" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B470" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C470" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D470" s="7"/>
       <c r="E470" s="7"/>
-      <c r="F470" s="7"/>
-      <c r="G470" s="7"/>
-    </row>
-    <row r="471" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A471" s="7"/>
-      <c r="B471" s="7"/>
-      <c r="C471" s="7"/>
+      <c r="F470" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="G470" s="7" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="471" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A471" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B471" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C471" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="D471" s="7"/>
       <c r="E471" s="7"/>
-      <c r="F471" s="7"/>
-      <c r="G471" s="7"/>
+      <c r="F471" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G471" s="7" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="472" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A472" s="7"/>
-      <c r="B472" s="7"/>
-      <c r="C472" s="7"/>
+      <c r="A472" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B472" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C472" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D472" s="7"/>
       <c r="E472" s="7"/>
-      <c r="F472" s="7"/>
-      <c r="G472" s="7"/>
-    </row>
-    <row r="473" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A473" s="7"/>
-      <c r="B473" s="7"/>
-      <c r="C473" s="7"/>
+      <c r="F472" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="G472" s="7" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="473" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A473" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B473" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C473" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D473" s="7"/>
       <c r="E473" s="7"/>
-      <c r="F473" s="7"/>
-      <c r="G473" s="7"/>
+      <c r="F473" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="G473" s="7" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="474" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A474" s="7"/>
-      <c r="B474" s="7"/>
-      <c r="C474" s="7"/>
+      <c r="A474" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B474" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C474" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D474" s="7"/>
       <c r="E474" s="7"/>
-      <c r="F474" s="7"/>
-      <c r="G474" s="7"/>
-    </row>
-    <row r="475" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A475" s="7"/>
-      <c r="B475" s="7"/>
-      <c r="C475" s="7"/>
+      <c r="F474" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="G474" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="475" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A475" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B475" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C475" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D475" s="7"/>
       <c r="E475" s="7"/>
-      <c r="F475" s="7"/>
-      <c r="G475" s="7"/>
+      <c r="F475" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="G475" s="7" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="476" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A476" s="7"/>
-      <c r="B476" s="7"/>
-      <c r="C476" s="7"/>
+      <c r="A476" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B476" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C476" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D476" s="7"/>
       <c r="E476" s="7"/>
-      <c r="F476" s="7"/>
-      <c r="G476" s="7"/>
-    </row>
-    <row r="477" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A477" s="7"/>
-      <c r="B477" s="7"/>
-      <c r="C477" s="7"/>
+      <c r="F476" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="G476" s="7" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="477" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A477" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B477" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C477" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D477" s="7"/>
       <c r="E477" s="7"/>
-      <c r="F477" s="7"/>
-      <c r="G477" s="7"/>
-    </row>
-    <row r="478" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A478" s="7"/>
-      <c r="B478" s="7"/>
-      <c r="C478" s="7"/>
+      <c r="F477" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="G477" s="7" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="478" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A478" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B478" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C478" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D478" s="7"/>
       <c r="E478" s="7"/>
-      <c r="F478" s="7"/>
-      <c r="G478" s="7"/>
+      <c r="F478" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="G478" s="7" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="479" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A479" s="7"/>
-      <c r="B479" s="7"/>
-      <c r="C479" s="7"/>
+      <c r="A479" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B479" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C479" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D479" s="7"/>
       <c r="E479" s="7"/>
-      <c r="F479" s="7"/>
-      <c r="G479" s="7"/>
-    </row>
-    <row r="480" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A480" s="7"/>
-      <c r="B480" s="7"/>
-      <c r="C480" s="7"/>
+      <c r="F479" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="G479" s="7" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="480" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A480" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B480" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C480" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D480" s="7"/>
       <c r="E480" s="7"/>
-      <c r="F480" s="7"/>
-      <c r="G480" s="7"/>
-    </row>
-    <row r="481" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A481" s="7"/>
-      <c r="B481" s="7"/>
-      <c r="C481" s="7"/>
+      <c r="F480" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="G480" s="7" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="481" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A481" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B481" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C481" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D481" s="7"/>
       <c r="E481" s="7"/>
-      <c r="F481" s="7"/>
-      <c r="G481" s="7"/>
+      <c r="F481" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="G481" s="7" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="482" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A482" s="7"/>
-      <c r="B482" s="7"/>
-      <c r="C482" s="7"/>
+      <c r="A482" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B482" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C482" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D482" s="7"/>
       <c r="E482" s="7"/>
-      <c r="F482" s="7"/>
-      <c r="G482" s="7"/>
-    </row>
-    <row r="483" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A483" s="7"/>
-      <c r="B483" s="7"/>
-      <c r="C483" s="7"/>
+      <c r="F482" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="G482" s="7" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="483" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A483" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B483" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C483" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D483" s="7"/>
       <c r="E483" s="7"/>
-      <c r="F483" s="7"/>
-      <c r="G483" s="7"/>
+      <c r="F483" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="G483" s="7" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="484" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A484" s="7"/>
-      <c r="B484" s="7"/>
-      <c r="C484" s="7"/>
+      <c r="A484" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B484" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C484" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D484" s="7"/>
       <c r="E484" s="7"/>
-      <c r="F484" s="7"/>
-      <c r="G484" s="7"/>
+      <c r="F484" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="G484" s="7" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="485" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A485" s="7"/>
-      <c r="B485" s="7"/>
-      <c r="C485" s="7"/>
+      <c r="A485" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B485" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C485" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D485" s="7"/>
       <c r="E485" s="7"/>
-      <c r="F485" s="7"/>
-      <c r="G485" s="7"/>
+      <c r="F485" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="G485" s="7" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="486" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A486" s="7"/>
-      <c r="B486" s="7"/>
-      <c r="C486" s="7"/>
+      <c r="A486" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B486" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C486" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D486" s="7"/>
       <c r="E486" s="7"/>
-      <c r="F486" s="7"/>
-      <c r="G486" s="7"/>
+      <c r="F486" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="G486" s="7" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="487" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A487" s="7"/>
-      <c r="B487" s="7"/>
-      <c r="C487" s="7"/>
+      <c r="A487" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B487" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C487" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D487" s="7"/>
       <c r="E487" s="7"/>
-      <c r="F487" s="7"/>
-      <c r="G487" s="7"/>
-    </row>
-    <row r="488" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A488" s="7"/>
-      <c r="B488" s="7"/>
-      <c r="C488" s="7"/>
+      <c r="F487" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="G487" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="488" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A488" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B488" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C488" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D488" s="7"/>
       <c r="E488" s="7"/>
-      <c r="F488" s="7"/>
-      <c r="G488" s="7"/>
-    </row>
-    <row r="489" spans="1:7" ht="29.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A489" s="7"/>
-      <c r="B489" s="7"/>
-      <c r="C489" s="7"/>
+      <c r="F488" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="G488" s="7" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="489" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A489" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B489" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C489" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D489" s="7"/>
       <c r="E489" s="7"/>
-      <c r="F489" s="7"/>
-      <c r="G489" s="7"/>
-    </row>
-    <row r="490" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A490" s="7"/>
-      <c r="B490" s="7"/>
-      <c r="C490" s="7"/>
+      <c r="F489" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="G489" s="7" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="490" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A490" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B490" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C490" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D490" s="7"/>
       <c r="E490" s="7"/>
-      <c r="F490" s="7"/>
-      <c r="G490" s="7"/>
-    </row>
-    <row r="491" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A491" s="7"/>
-      <c r="B491" s="7"/>
-      <c r="C491" s="7"/>
+      <c r="F490" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="G490" s="7" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="491" spans="1:7" ht="29.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A491" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B491" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C491" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D491" s="7"/>
       <c r="E491" s="7"/>
-      <c r="F491" s="7"/>
-      <c r="G491" s="7"/>
+      <c r="F491" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="G491" s="7" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="492" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A492" s="7"/>
-      <c r="B492" s="7"/>
-      <c r="C492" s="7"/>
+      <c r="A492" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B492" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C492" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D492" s="7"/>
       <c r="E492" s="7"/>
-      <c r="F492" s="7"/>
-      <c r="G492" s="7"/>
-    </row>
-    <row r="493" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A493" s="7"/>
-      <c r="B493" s="7"/>
-      <c r="C493" s="7"/>
+      <c r="F492" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="G492" s="7" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="493" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A493" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B493" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C493" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D493" s="7"/>
       <c r="E493" s="7"/>
-      <c r="F493" s="7"/>
-      <c r="G493" s="7"/>
-    </row>
-    <row r="494" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A494" s="8"/>
-      <c r="B494" s="8"/>
-      <c r="C494" s="8"/>
-      <c r="D494" s="8"/>
-      <c r="E494" s="8"/>
-      <c r="F494" s="8"/>
-      <c r="G494" s="8"/>
+      <c r="F493" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="G493" s="7" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="494" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A494" s="7"/>
+      <c r="B494" s="7"/>
+      <c r="C494" s="7"/>
+      <c r="D494" s="7"/>
+      <c r="E494" s="7"/>
+      <c r="F494" s="7"/>
+      <c r="G494" s="7"/>
     </row>
     <row r="495" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A495" s="8"/>
-      <c r="B495" s="8"/>
-      <c r="C495" s="8"/>
-      <c r="D495" s="8"/>
-      <c r="E495" s="8"/>
-      <c r="F495" s="8"/>
-      <c r="G495" s="8"/>
-    </row>
-    <row r="496" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A495" s="7"/>
+      <c r="B495" s="7"/>
+      <c r="C495" s="7"/>
+      <c r="D495" s="7"/>
+      <c r="E495" s="7"/>
+      <c r="F495" s="7"/>
+      <c r="G495" s="7"/>
+    </row>
+    <row r="496" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A496" s="8"/>
       <c r="B496" s="8"/>
       <c r="C496" s="8"/>
@@ -11000,7 +11570,7 @@
       <c r="F496" s="8"/>
       <c r="G496" s="8"/>
     </row>
-    <row r="497" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="497" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A497" s="8"/>
       <c r="B497" s="8"/>
       <c r="C497" s="8"/>
@@ -11018,7 +11588,7 @@
       <c r="F498" s="8"/>
       <c r="G498" s="8"/>
     </row>
-    <row r="499" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="499" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A499" s="8"/>
       <c r="B499" s="8"/>
       <c r="C499" s="8"/>
@@ -11063,7 +11633,7 @@
       <c r="F503" s="8"/>
       <c r="G503" s="8"/>
     </row>
-    <row r="504" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="504" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A504" s="8"/>
       <c r="B504" s="8"/>
       <c r="C504" s="8"/>
@@ -11081,7 +11651,7 @@
       <c r="F505" s="8"/>
       <c r="G505" s="8"/>
     </row>
-    <row r="506" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="506" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A506" s="8"/>
       <c r="B506" s="8"/>
       <c r="C506" s="8"/>
@@ -11090,7 +11660,7 @@
       <c r="F506" s="8"/>
       <c r="G506" s="8"/>
     </row>
-    <row r="507" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="507" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A507" s="8"/>
       <c r="B507" s="8"/>
       <c r="C507" s="8"/>
@@ -11108,7 +11678,7 @@
       <c r="F508" s="8"/>
       <c r="G508" s="8"/>
     </row>
-    <row r="509" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="509" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A509" s="8"/>
       <c r="B509" s="8"/>
       <c r="C509" s="8"/>
@@ -11117,7 +11687,7 @@
       <c r="F509" s="8"/>
       <c r="G509" s="8"/>
     </row>
-    <row r="510" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="510" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A510" s="8"/>
       <c r="B510" s="8"/>
       <c r="C510" s="8"/>
@@ -11135,7 +11705,7 @@
       <c r="F511" s="8"/>
       <c r="G511" s="8"/>
     </row>
-    <row r="512" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="512" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A512" s="8"/>
       <c r="B512" s="8"/>
       <c r="C512" s="8"/>
@@ -11153,7 +11723,7 @@
       <c r="F513" s="8"/>
       <c r="G513" s="8"/>
     </row>
-    <row r="514" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="514" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A514" s="8"/>
       <c r="B514" s="8"/>
       <c r="C514" s="8"/>
@@ -11171,7 +11741,7 @@
       <c r="F515" s="8"/>
       <c r="G515" s="8"/>
     </row>
-    <row r="516" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="516" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A516" s="8"/>
       <c r="B516" s="8"/>
       <c r="C516" s="8"/>
@@ -11180,7 +11750,7 @@
       <c r="F516" s="8"/>
       <c r="G516" s="8"/>
     </row>
-    <row r="517" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="517" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A517" s="8"/>
       <c r="B517" s="8"/>
       <c r="C517" s="8"/>
@@ -11198,7 +11768,7 @@
       <c r="F518" s="8"/>
       <c r="G518" s="8"/>
     </row>
-    <row r="519" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="519" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A519" s="8"/>
       <c r="B519" s="8"/>
       <c r="C519" s="8"/>
@@ -11252,7 +11822,7 @@
       <c r="F524" s="8"/>
       <c r="G524" s="8"/>
     </row>
-    <row r="525" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="525" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A525" s="8"/>
       <c r="B525" s="8"/>
       <c r="C525" s="8"/>
@@ -11261,7 +11831,7 @@
       <c r="F525" s="8"/>
       <c r="G525" s="8"/>
     </row>
-    <row r="526" spans="1:7" ht="29.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="526" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A526" s="8"/>
       <c r="B526" s="8"/>
       <c r="C526" s="8"/>
@@ -11270,7 +11840,7 @@
       <c r="F526" s="8"/>
       <c r="G526" s="8"/>
     </row>
-    <row r="527" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="527" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A527" s="8"/>
       <c r="B527" s="8"/>
       <c r="C527" s="8"/>
@@ -11279,7 +11849,7 @@
       <c r="F527" s="8"/>
       <c r="G527" s="8"/>
     </row>
-    <row r="528" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="528" spans="1:7" ht="29.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A528" s="8"/>
       <c r="B528" s="8"/>
       <c r="C528" s="8"/>
@@ -11288,24 +11858,26 @@
       <c r="F528" s="8"/>
       <c r="G528" s="8"/>
     </row>
-    <row r="591" spans="6:6" x14ac:dyDescent="0.4">
-      <c r="F591" s="7"/>
-    </row>
-    <row r="638" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A638" s="8"/>
-      <c r="B638" s="10"/>
-      <c r="C638" s="10"/>
-      <c r="D638" s="10"/>
-      <c r="E638" s="10"/>
-      <c r="F638" s="10"/>
-    </row>
-    <row r="639" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A639" s="8"/>
-      <c r="B639" s="10"/>
-      <c r="C639" s="10"/>
-      <c r="D639" s="10"/>
-      <c r="E639" s="10"/>
-      <c r="F639" s="10"/>
+    <row r="529" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A529" s="8"/>
+      <c r="B529" s="8"/>
+      <c r="C529" s="8"/>
+      <c r="D529" s="8"/>
+      <c r="E529" s="8"/>
+      <c r="F529" s="8"/>
+      <c r="G529" s="8"/>
+    </row>
+    <row r="530" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A530" s="8"/>
+      <c r="B530" s="8"/>
+      <c r="C530" s="8"/>
+      <c r="D530" s="8"/>
+      <c r="E530" s="8"/>
+      <c r="F530" s="8"/>
+      <c r="G530" s="8"/>
+    </row>
+    <row r="593" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F593" s="7"/>
     </row>
     <row r="640" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A640" s="8"/>
@@ -11423,7 +11995,7 @@
       <c r="A654" s="8"/>
       <c r="B654" s="10"/>
       <c r="C654" s="10"/>
-      <c r="D654" s="8"/>
+      <c r="D654" s="10"/>
       <c r="E654" s="10"/>
       <c r="F654" s="10"/>
     </row>
@@ -11431,7 +12003,7 @@
       <c r="A655" s="8"/>
       <c r="B655" s="10"/>
       <c r="C655" s="10"/>
-      <c r="D655" s="8"/>
+      <c r="D655" s="10"/>
       <c r="E655" s="10"/>
       <c r="F655" s="10"/>
     </row>
@@ -11483,21 +12055,21 @@
       <c r="E661" s="10"/>
       <c r="F661" s="10"/>
     </row>
-    <row r="715" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A715" s="11"/>
-      <c r="B715" s="11"/>
-      <c r="C715" s="11"/>
-      <c r="D715" s="11"/>
-      <c r="E715" s="11"/>
-      <c r="F715" s="11"/>
-    </row>
-    <row r="716" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A716" s="11"/>
-      <c r="B716" s="11"/>
-      <c r="C716" s="11"/>
-      <c r="D716" s="11"/>
-      <c r="E716" s="11"/>
-      <c r="F716" s="11"/>
+    <row r="662" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A662" s="8"/>
+      <c r="B662" s="10"/>
+      <c r="C662" s="10"/>
+      <c r="D662" s="8"/>
+      <c r="E662" s="10"/>
+      <c r="F662" s="10"/>
+    </row>
+    <row r="663" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A663" s="8"/>
+      <c r="B663" s="10"/>
+      <c r="C663" s="10"/>
+      <c r="D663" s="8"/>
+      <c r="E663" s="10"/>
+      <c r="F663" s="10"/>
     </row>
     <row r="717" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A717" s="11"/>
@@ -11737,7 +12309,7 @@
       <c r="C746" s="11"/>
       <c r="D746" s="11"/>
       <c r="E746" s="11"/>
-      <c r="F746" s="12"/>
+      <c r="F746" s="11"/>
     </row>
     <row r="747" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A747" s="11"/>
@@ -11769,7 +12341,7 @@
       <c r="C750" s="11"/>
       <c r="D750" s="11"/>
       <c r="E750" s="11"/>
-      <c r="F750" s="11"/>
+      <c r="F750" s="12"/>
     </row>
     <row r="751" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A751" s="11"/>
@@ -12051,24 +12623,30 @@
       <c r="E785" s="11"/>
       <c r="F785" s="11"/>
     </row>
-    <row r="794" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="795" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A795" s="4"/>
-      <c r="B795" s="4"/>
-    </row>
-    <row r="796" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A796" s="4"/>
-      <c r="B796" s="4"/>
-    </row>
-    <row r="811" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D811" s="3"/>
-      <c r="E811" s="3"/>
-      <c r="F811" s="3"/>
-    </row>
-    <row r="812" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D812" s="3"/>
-      <c r="E812" s="3"/>
-      <c r="F812" s="3"/>
+    <row r="786" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A786" s="11"/>
+      <c r="B786" s="11"/>
+      <c r="C786" s="11"/>
+      <c r="D786" s="11"/>
+      <c r="E786" s="11"/>
+      <c r="F786" s="11"/>
+    </row>
+    <row r="787" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A787" s="11"/>
+      <c r="B787" s="11"/>
+      <c r="C787" s="11"/>
+      <c r="D787" s="11"/>
+      <c r="E787" s="11"/>
+      <c r="F787" s="11"/>
+    </row>
+    <row r="796" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="797" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A797" s="4"/>
+      <c r="B797" s="4"/>
+    </row>
+    <row r="798" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A798" s="4"/>
+      <c r="B798" s="4"/>
     </row>
     <row r="813" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D813" s="3"/>
@@ -12205,23 +12783,15 @@
       <c r="E839" s="3"/>
       <c r="F839" s="3"/>
     </row>
-    <row r="840" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A840" s="8"/>
-      <c r="B840" s="10"/>
-      <c r="C840" s="10"/>
-      <c r="D840" s="10"/>
-      <c r="E840" s="10"/>
-      <c r="F840" s="10"/>
-      <c r="G840" s="8"/>
-    </row>
-    <row r="841" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A841" s="8"/>
-      <c r="B841" s="10"/>
-      <c r="C841" s="10"/>
-      <c r="D841" s="10"/>
-      <c r="E841" s="10"/>
-      <c r="F841" s="10"/>
-      <c r="G841" s="8"/>
+    <row r="840" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D840" s="3"/>
+      <c r="E840" s="3"/>
+      <c r="F840" s="3"/>
+    </row>
+    <row r="841" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D841" s="3"/>
+      <c r="E841" s="3"/>
+      <c r="F841" s="3"/>
     </row>
     <row r="842" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A842" s="8"/>
@@ -12395,21 +12965,21 @@
       <c r="G860" s="8"/>
     </row>
     <row r="861" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A861" s="5"/>
-      <c r="B861" s="8"/>
-      <c r="C861" s="8"/>
-      <c r="D861" s="8"/>
-      <c r="E861" s="8"/>
-      <c r="F861" s="8"/>
+      <c r="A861" s="8"/>
+      <c r="B861" s="10"/>
+      <c r="C861" s="10"/>
+      <c r="D861" s="10"/>
+      <c r="E861" s="10"/>
+      <c r="F861" s="10"/>
       <c r="G861" s="8"/>
     </row>
     <row r="862" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A862" s="5"/>
-      <c r="B862" s="8"/>
-      <c r="C862" s="8"/>
-      <c r="D862" s="8"/>
-      <c r="E862" s="8"/>
-      <c r="F862" s="8"/>
+      <c r="A862" s="8"/>
+      <c r="B862" s="10"/>
+      <c r="C862" s="10"/>
+      <c r="D862" s="10"/>
+      <c r="E862" s="10"/>
+      <c r="F862" s="10"/>
       <c r="G862" s="8"/>
     </row>
     <row r="863" spans="1:7" x14ac:dyDescent="0.4">
@@ -12534,7 +13104,7 @@
       <c r="B876" s="8"/>
       <c r="C876" s="8"/>
       <c r="D876" s="8"/>
-      <c r="E876" s="10"/>
+      <c r="E876" s="8"/>
       <c r="F876" s="8"/>
       <c r="G876" s="8"/>
     </row>
@@ -12543,7 +13113,7 @@
       <c r="B877" s="8"/>
       <c r="C877" s="8"/>
       <c r="D877" s="8"/>
-      <c r="E877" s="10"/>
+      <c r="E877" s="8"/>
       <c r="F877" s="8"/>
       <c r="G877" s="8"/>
     </row>
@@ -13014,6 +13584,24 @@
       <c r="E929" s="10"/>
       <c r="F929" s="8"/>
       <c r="G929" s="8"/>
+    </row>
+    <row r="930" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A930" s="5"/>
+      <c r="B930" s="8"/>
+      <c r="C930" s="8"/>
+      <c r="D930" s="8"/>
+      <c r="E930" s="10"/>
+      <c r="F930" s="8"/>
+      <c r="G930" s="8"/>
+    </row>
+    <row r="931" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A931" s="5"/>
+      <c r="B931" s="8"/>
+      <c r="C931" s="8"/>
+      <c r="D931" s="8"/>
+      <c r="E931" s="10"/>
+      <c r="F931" s="8"/>
+      <c r="G931" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>